<commit_message>
eddy ni 1979-1980 (update)
</commit_message>
<xml_diff>
--- a/_data/ni/ni7980/individueel_eindstand_dworp_12_7980.xlsx
+++ b/_data/ni/ni7980/individueel_eindstand_dworp_12_7980.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="177">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Baekeland Pieter</t>
   </si>
   <si>
-    <t>719 Waterschei</t>
-  </si>
-  <si>
     <t>Krivitzki H</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>Janssens Fritz</t>
   </si>
   <si>
-    <t>245 Caïssa Ganshoren</t>
-  </si>
-  <si>
     <t>Joseph Fernand</t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>Noseda JM</t>
   </si>
   <si>
-    <t>238 Zaventem</t>
-  </si>
-  <si>
     <t>Van Damme F</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
   </si>
   <si>
     <t>Schols Joël</t>
-  </si>
-  <si>
-    <t>203 Fous du Roy</t>
   </si>
   <si>
     <t>Devos P</t>
@@ -298,9 +286,6 @@
     <t>Dewasseige A</t>
   </si>
   <si>
-    <t>20165 Waterloo</t>
-  </si>
-  <si>
     <t>Marinof M</t>
   </si>
   <si>
@@ -311,9 +296,6 @@
   </si>
   <si>
     <t>Delmarbol</t>
-  </si>
-  <si>
-    <t>244 Thibaut</t>
   </si>
   <si>
     <t>Thibaut Georges</t>
@@ -332,9 +314,6 @@
   </si>
   <si>
     <t>Bottu E</t>
-  </si>
-  <si>
-    <t>707 Tessenderlo</t>
   </si>
   <si>
     <t>De Wel M</t>
@@ -403,9 +382,6 @@
     <t>blinde vlek</t>
   </si>
   <si>
-    <t>234 Le Mat</t>
-  </si>
-  <si>
     <t>Reinitz A</t>
   </si>
   <si>
@@ -434,9 +410,6 @@
   </si>
   <si>
     <t>Jatidjan R</t>
-  </si>
-  <si>
-    <t>CRE Charleroi 2</t>
   </si>
   <si>
     <t>Havelange P</t>
@@ -490,9 +463,6 @@
     <t>Pauwels D</t>
   </si>
   <si>
-    <t xml:space="preserve">418 Geraardsbergen </t>
-  </si>
-  <si>
     <t>Flamée Dirk</t>
   </si>
   <si>
@@ -526,64 +496,7 @@
     <t>Wasnaire A</t>
   </si>
   <si>
-    <t>Fous du Roi 1</t>
-  </si>
-  <si>
-    <t>Queen Caïssa Ganshoren 1</t>
-  </si>
-  <si>
-    <t>Thibaut 1</t>
-  </si>
-  <si>
-    <t>Soignies</t>
-  </si>
-  <si>
-    <t>Geraardsbergen</t>
-  </si>
-  <si>
-    <t>Gligoric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRE Charleroi </t>
-  </si>
-  <si>
     <t>Morphy</t>
-  </si>
-  <si>
-    <t>Jean Jaurès</t>
-  </si>
-  <si>
-    <t>Waterloo 1</t>
-  </si>
-  <si>
-    <t>Tessenderlo 1</t>
-  </si>
-  <si>
-    <t>Geraardsbergen 2</t>
-  </si>
-  <si>
-    <t>Leuven 2</t>
-  </si>
-  <si>
-    <t>Zaventem 1</t>
-  </si>
-  <si>
-    <t>Wavre 2</t>
-  </si>
-  <si>
-    <t>Le Mat 4</t>
-  </si>
-  <si>
-    <t>Waterschei 1</t>
-  </si>
-  <si>
-    <t>Drogon Bleu</t>
-  </si>
-  <si>
-    <t>Ech. Anderlecht 1</t>
-  </si>
-  <si>
-    <t>Ruisbroek 2</t>
   </si>
   <si>
     <t>90(27)</t>
@@ -607,10 +520,43 @@
     <t>D1: vier ploeguitslagen ontbreken, aangeduid als blinde vlek</t>
   </si>
   <si>
-    <t>3x</t>
+    <t>3X</t>
   </si>
   <si>
-    <t>4x</t>
+    <t>4X</t>
+  </si>
+  <si>
+    <t>719 Waterschei 1</t>
+  </si>
+  <si>
+    <t>245 Queen Caïssa Ganshoren 1</t>
+  </si>
+  <si>
+    <t>238 Zaventem 1</t>
+  </si>
+  <si>
+    <t>244 Thibaut 1</t>
+  </si>
+  <si>
+    <t>707 Tessenderlo 1</t>
+  </si>
+  <si>
+    <t>418 Geraardsbergen 2</t>
+  </si>
+  <si>
+    <t>234 Le Mat 4</t>
+  </si>
+  <si>
+    <t>203 Fous du Roy 1</t>
+  </si>
+  <si>
+    <t>501 CRE Charleroi 2</t>
+  </si>
+  <si>
+    <t>402 Jean Jaurès Gent</t>
+  </si>
+  <si>
+    <t>216 Waterloo 1</t>
   </si>
 </sst>
 </file>
@@ -1762,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="D5" s="68" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="G5" s="68"/>
       <c r="H5" s="68"/>
@@ -1779,13 +1725,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="D6" s="68" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="G6" s="68"/>
       <c r="H6" s="68"/>
@@ -1797,7 +1743,7 @@
       </c>
       <c r="B7" s="29"/>
       <c r="F7" s="74" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="74"/>
@@ -1811,7 +1757,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="D10" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
@@ -1821,7 +1767,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="D11" s="71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="71"/>
       <c r="F11" s="71"/>
@@ -1831,7 +1777,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="D13" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="5:6">
@@ -1848,7 +1794,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1888,7 +1834,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1938,7 +1884,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -1966,7 +1912,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -1994,7 +1940,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -2022,7 +1968,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -2050,7 +1996,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -2072,7 +2018,7 @@
         <v>1708</v>
       </c>
       <c r="L9" s="69" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1">
@@ -2081,7 +2027,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -2097,7 +2043,7 @@
         <v>57282</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="18">
         <v>1450</v>
@@ -2148,7 +2094,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2206,7 +2152,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -2234,7 +2180,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -2262,7 +2208,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -2290,7 +2236,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -2653,7 +2599,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2813,7 +2759,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2863,7 +2809,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -2891,7 +2837,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -2919,7 +2865,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -2947,7 +2893,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -3274,7 +3220,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:D18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3314,7 +3260,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3364,7 +3310,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -3392,7 +3338,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -3420,7 +3366,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -3448,7 +3394,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -3476,7 +3422,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -3504,7 +3450,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -3571,7 +3517,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -3629,7 +3575,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -3641,7 +3587,7 @@
         <v>57282</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="18">
         <v>1450</v>
@@ -3657,7 +3603,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -3685,7 +3631,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -3713,7 +3659,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -4022,7 +3968,7 @@
   <dimension ref="A1:AQ280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4030,7 +3976,7 @@
     <col min="1" max="1" width="3" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" style="31" customWidth="1"/>
     <col min="3" max="14" width="4" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="31" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.42578125" style="31" customWidth="1"/>
     <col min="17" max="17" width="4.28515625" style="31" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="31"/>
@@ -4149,15 +4095,14 @@
       <c r="M4" s="41"/>
       <c r="N4" s="41"/>
       <c r="O4" s="42">
-        <f t="shared" ref="O4:O15" si="1">SUM(C4:N4)</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="P4" s="43">
         <f>SUM(S4:AD4)*2</f>
         <v>0</v>
       </c>
       <c r="Q4" s="43">
-        <f t="shared" ref="Q4:Q15" si="2">COUNT(C4:N4)</f>
+        <f t="shared" ref="Q4:Q15" si="1">COUNT(C4:N4)</f>
         <v>0</v>
       </c>
       <c r="R4" s="72">
@@ -4263,7 +4208,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="40" t="s">
@@ -4280,15 +4225,14 @@
       <c r="M5" s="41"/>
       <c r="N5" s="41"/>
       <c r="O5" s="42">
+        <v>92</v>
+      </c>
+      <c r="P5" s="43">
+        <f t="shared" ref="P5:P15" si="2">SUM(S5:AD5)*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="43">
-        <f t="shared" ref="P5:P15" si="3">SUM(S5:AD5)*2</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R5" s="72">
@@ -4394,7 +4338,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -4411,15 +4355,14 @@
       <c r="M6" s="41"/>
       <c r="N6" s="41"/>
       <c r="O6" s="42">
+        <v>91</v>
+      </c>
+      <c r="P6" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R6" s="72">
@@ -4525,7 +4468,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -4542,15 +4485,14 @@
       <c r="M7" s="41"/>
       <c r="N7" s="41"/>
       <c r="O7" s="42">
+        <v>89</v>
+      </c>
+      <c r="P7" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R7" s="72">
@@ -4656,7 +4598,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>170</v>
+        <v>52</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
@@ -4673,15 +4615,14 @@
       <c r="M8" s="41"/>
       <c r="N8" s="41"/>
       <c r="O8" s="42">
+        <v>79</v>
+      </c>
+      <c r="P8" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R8" s="72">
@@ -4787,7 +4728,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
@@ -4804,15 +4745,14 @@
       <c r="M9" s="41"/>
       <c r="N9" s="41"/>
       <c r="O9" s="42">
+        <v>77</v>
+      </c>
+      <c r="P9" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R9" s="72">
@@ -4918,7 +4858,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -4935,15 +4875,14 @@
       <c r="M10" s="41"/>
       <c r="N10" s="41"/>
       <c r="O10" s="42">
+        <v>67</v>
+      </c>
+      <c r="P10" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R10" s="72">
@@ -5049,7 +4988,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
@@ -5066,15 +5005,14 @@
       <c r="M11" s="41"/>
       <c r="N11" s="41"/>
       <c r="O11" s="42">
+        <v>66</v>
+      </c>
+      <c r="P11" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R11" s="72">
@@ -5180,7 +5118,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
@@ -5197,19 +5135,19 @@
       <c r="M12" s="41"/>
       <c r="N12" s="41"/>
       <c r="O12" s="42">
+        <f t="shared" ref="O4:O15" si="3">SUM(C12:N12)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P12" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="R12" s="73" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="S12" s="54" t="str">
         <f>IF(C12="","",IF(C12&gt;$K4,1,IF(C12=$K4,0.5,0)))</f>
@@ -5311,7 +5249,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -5328,19 +5266,19 @@
       <c r="M13" s="41"/>
       <c r="N13" s="41"/>
       <c r="O13" s="42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P13" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="R13" s="73" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="S13" s="54" t="str">
         <f>IF(C13="","",IF(C13&gt;$L4,1,IF(C13=$L4,0.5,0)))</f>
@@ -5457,15 +5395,15 @@
       </c>
       <c r="N14" s="41"/>
       <c r="O14" s="42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="43">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R14" s="52"/>
@@ -5584,15 +5522,15 @@
         <v>37</v>
       </c>
       <c r="O15" s="48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="49">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="49">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R15" s="52"/>
@@ -5790,7 +5728,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>37</v>
@@ -5807,15 +5745,14 @@
       <c r="M18" s="41"/>
       <c r="N18" s="41"/>
       <c r="O18" s="42">
-        <f t="shared" ref="O18:O29" si="16">SUM(C18:N18)</f>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="P18" s="43">
         <f>SUM(S18:AD18)*2</f>
         <v>0</v>
       </c>
       <c r="Q18" s="43">
-        <f t="shared" ref="Q18:Q29" si="17">COUNT(C18:N18)</f>
+        <f t="shared" ref="Q18:Q29" si="16">COUNT(C18:N18)</f>
         <v>0</v>
       </c>
       <c r="R18" s="72">
@@ -5921,7 +5858,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="40" t="s">
@@ -5938,15 +5875,14 @@
       <c r="M19" s="41"/>
       <c r="N19" s="41"/>
       <c r="O19" s="42">
+        <v>102</v>
+      </c>
+      <c r="P19" s="43">
+        <f t="shared" ref="P19:P29" si="17">SUM(S19:AD19)*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="43">
-        <f t="shared" ref="P19:P29" si="18">SUM(S19:AD19)*2</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R19" s="72">
@@ -6052,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
@@ -6069,15 +6005,14 @@
       <c r="M20" s="41"/>
       <c r="N20" s="41"/>
       <c r="O20" s="42">
+        <v>96</v>
+      </c>
+      <c r="P20" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R20" s="72">
@@ -6183,7 +6118,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>178</v>
+        <v>123</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
@@ -6200,15 +6135,14 @@
       <c r="M21" s="41"/>
       <c r="N21" s="41"/>
       <c r="O21" s="42">
+        <v>95</v>
+      </c>
+      <c r="P21" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R21" s="72">
@@ -6314,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -6331,15 +6265,14 @@
       <c r="M22" s="41"/>
       <c r="N22" s="41"/>
       <c r="O22" s="42">
+        <v>91</v>
+      </c>
+      <c r="P22" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R22" s="72">
@@ -6445,7 +6378,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
@@ -6462,19 +6395,17 @@
       <c r="M23" s="41"/>
       <c r="N23" s="41"/>
       <c r="O23" s="42">
+        <v>90</v>
+      </c>
+      <c r="P23" s="43">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="43">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="P23" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="43">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
       <c r="R23" s="73" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="S23" s="54" t="str">
         <f>IF(C23="","",IF(C23&gt;$H18,1,IF(C23=$H18,0.5,0)))</f>
@@ -6576,7 +6507,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
@@ -6593,19 +6524,17 @@
       <c r="M24" s="41"/>
       <c r="N24" s="41"/>
       <c r="O24" s="42">
+        <v>90</v>
+      </c>
+      <c r="P24" s="43">
+        <v>23</v>
+      </c>
+      <c r="Q24" s="43">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="P24" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="43">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
       <c r="R24" s="73" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="S24" s="54" t="str">
         <f>IF(C24="","",IF(C24&gt;$I18,1,IF(C24=$I18,0.5,0)))</f>
@@ -6707,7 +6636,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
@@ -6724,19 +6653,17 @@
       <c r="M25" s="41"/>
       <c r="N25" s="41"/>
       <c r="O25" s="42">
+        <v>90</v>
+      </c>
+      <c r="P25" s="43">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="43">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="P25" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="43">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
       <c r="R25" s="73" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="S25" s="54" t="str">
         <f>IF(C25="","",IF(C25&gt;$J18,1,IF(C25=$J18,0.5,0)))</f>
@@ -6838,7 +6765,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -6855,15 +6782,14 @@
       <c r="M26" s="41"/>
       <c r="N26" s="41"/>
       <c r="O26" s="42">
+        <v>89</v>
+      </c>
+      <c r="P26" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R26" s="72">
@@ -6969,7 +6895,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -6986,15 +6912,14 @@
       <c r="M27" s="41"/>
       <c r="N27" s="41"/>
       <c r="O27" s="42">
+        <v>71</v>
+      </c>
+      <c r="P27" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R27" s="72">
@@ -7100,7 +7025,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
@@ -7117,15 +7042,14 @@
       </c>
       <c r="N28" s="41"/>
       <c r="O28" s="42">
+        <v>64</v>
+      </c>
+      <c r="P28" s="43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="43">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="43">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R28" s="72">
@@ -7231,7 +7155,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>185</v>
+        <v>112</v>
       </c>
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
@@ -7248,15 +7172,14 @@
         <v>37</v>
       </c>
       <c r="O29" s="48">
+        <v>56</v>
+      </c>
+      <c r="P29" s="49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="49">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="49">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="49">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R29" s="72">
@@ -7382,51 +7305,51 @@
         <v>33</v>
       </c>
       <c r="C31" s="35">
-        <f t="shared" ref="C31" si="19">MATCH("XX",C32:C43,0)</f>
+        <f t="shared" ref="C31" si="18">MATCH("XX",C32:C43,0)</f>
         <v>1</v>
       </c>
       <c r="D31" s="35">
-        <f t="shared" ref="D31" si="20">MATCH("XX",D32:D43,0)</f>
+        <f t="shared" ref="D31" si="19">MATCH("XX",D32:D43,0)</f>
         <v>2</v>
       </c>
       <c r="E31" s="35">
-        <f t="shared" ref="E31" si="21">MATCH("XX",E32:E43,0)</f>
+        <f t="shared" ref="E31" si="20">MATCH("XX",E32:E43,0)</f>
         <v>3</v>
       </c>
       <c r="F31" s="35">
-        <f t="shared" ref="F31" si="22">MATCH("XX",F32:F43,0)</f>
+        <f t="shared" ref="F31" si="21">MATCH("XX",F32:F43,0)</f>
         <v>4</v>
       </c>
       <c r="G31" s="35">
-        <f t="shared" ref="G31" si="23">MATCH("XX",G32:G43,0)</f>
+        <f t="shared" ref="G31" si="22">MATCH("XX",G32:G43,0)</f>
         <v>5</v>
       </c>
       <c r="H31" s="35">
-        <f t="shared" ref="H31" si="24">MATCH("XX",H32:H43,0)</f>
+        <f t="shared" ref="H31" si="23">MATCH("XX",H32:H43,0)</f>
         <v>6</v>
       </c>
       <c r="I31" s="35">
-        <f t="shared" ref="I31" si="25">MATCH("XX",I32:I43,0)</f>
+        <f t="shared" ref="I31" si="24">MATCH("XX",I32:I43,0)</f>
         <v>7</v>
       </c>
       <c r="J31" s="35">
-        <f t="shared" ref="J31" si="26">MATCH("XX",J32:J43,0)</f>
+        <f t="shared" ref="J31" si="25">MATCH("XX",J32:J43,0)</f>
         <v>8</v>
       </c>
       <c r="K31" s="35">
-        <f t="shared" ref="K31" si="27">MATCH("XX",K32:K43,0)</f>
+        <f t="shared" ref="K31" si="26">MATCH("XX",K32:K43,0)</f>
         <v>9</v>
       </c>
       <c r="L31" s="35">
-        <f t="shared" ref="L31" si="28">MATCH("XX",L32:L43,0)</f>
+        <f t="shared" ref="L31" si="27">MATCH("XX",L32:L43,0)</f>
         <v>10</v>
       </c>
       <c r="M31" s="35">
-        <f t="shared" ref="M31" si="29">MATCH("XX",M32:M43,0)</f>
+        <f t="shared" ref="M31" si="28">MATCH("XX",M32:M43,0)</f>
         <v>11</v>
       </c>
       <c r="N31" s="35">
-        <f t="shared" ref="N31" si="30">MATCH("XX",N32:N43,0)</f>
+        <f t="shared" ref="N31" si="29">MATCH("XX",N32:N43,0)</f>
         <v>12</v>
       </c>
       <c r="O31" s="36" t="s">
@@ -7471,7 +7394,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="41"/>
       <c r="O32" s="42">
-        <f t="shared" ref="O32:O43" si="31">SUM(C32:N32)</f>
+        <f t="shared" ref="O32:O43" si="30">SUM(C32:N32)</f>
         <v>0</v>
       </c>
       <c r="P32" s="43">
@@ -7479,7 +7402,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="43">
-        <f t="shared" ref="Q32:Q43" si="32">COUNT(C32:N32)</f>
+        <f t="shared" ref="Q32:Q43" si="31">COUNT(C32:N32)</f>
         <v>0</v>
       </c>
       <c r="R32" s="52"/>
@@ -7598,15 +7521,15 @@
       <c r="M33" s="41"/>
       <c r="N33" s="41"/>
       <c r="O33" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="43">
+        <f t="shared" ref="P33:P43" si="32">SUM(S33:AD33)*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P33" s="43">
-        <f t="shared" ref="P33:P43" si="33">SUM(S33:AD33)*2</f>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R33" s="52"/>
@@ -7725,15 +7648,15 @@
       <c r="M34" s="41"/>
       <c r="N34" s="41"/>
       <c r="O34" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P34" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R34" s="52"/>
@@ -7852,15 +7775,15 @@
       <c r="M35" s="41"/>
       <c r="N35" s="41"/>
       <c r="O35" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R35" s="52"/>
@@ -7979,15 +7902,15 @@
       <c r="M36" s="41"/>
       <c r="N36" s="41"/>
       <c r="O36" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R36" s="52"/>
@@ -8106,15 +8029,15 @@
       <c r="M37" s="41"/>
       <c r="N37" s="41"/>
       <c r="O37" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R37" s="52"/>
@@ -8233,15 +8156,15 @@
       <c r="M38" s="41"/>
       <c r="N38" s="41"/>
       <c r="O38" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R38" s="52"/>
@@ -8360,15 +8283,15 @@
       <c r="M39" s="41"/>
       <c r="N39" s="41"/>
       <c r="O39" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R39" s="52"/>
@@ -8487,15 +8410,15 @@
       <c r="M40" s="41"/>
       <c r="N40" s="41"/>
       <c r="O40" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P40" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R40" s="52"/>
@@ -8614,15 +8537,15 @@
       <c r="M41" s="41"/>
       <c r="N41" s="41"/>
       <c r="O41" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P41" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q41" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R41" s="52"/>
@@ -8741,15 +8664,15 @@
       </c>
       <c r="N42" s="41"/>
       <c r="O42" s="42">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="43">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="43">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P42" s="43">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="43">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R42" s="52"/>
@@ -8868,15 +8791,15 @@
         <v>37</v>
       </c>
       <c r="O43" s="48">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="49">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="49">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="49">
-        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R43" s="52"/>
@@ -9000,51 +8923,51 @@
         <v>33</v>
       </c>
       <c r="C45" s="35">
-        <f t="shared" ref="C45" si="34">MATCH("XX",C46:C57,0)</f>
+        <f t="shared" ref="C45" si="33">MATCH("XX",C46:C57,0)</f>
         <v>1</v>
       </c>
       <c r="D45" s="35">
-        <f t="shared" ref="D45" si="35">MATCH("XX",D46:D57,0)</f>
+        <f t="shared" ref="D45" si="34">MATCH("XX",D46:D57,0)</f>
         <v>2</v>
       </c>
       <c r="E45" s="35">
-        <f t="shared" ref="E45" si="36">MATCH("XX",E46:E57,0)</f>
+        <f t="shared" ref="E45" si="35">MATCH("XX",E46:E57,0)</f>
         <v>3</v>
       </c>
       <c r="F45" s="35">
-        <f t="shared" ref="F45" si="37">MATCH("XX",F46:F57,0)</f>
+        <f t="shared" ref="F45" si="36">MATCH("XX",F46:F57,0)</f>
         <v>4</v>
       </c>
       <c r="G45" s="35">
-        <f t="shared" ref="G45" si="38">MATCH("XX",G46:G57,0)</f>
+        <f t="shared" ref="G45" si="37">MATCH("XX",G46:G57,0)</f>
         <v>5</v>
       </c>
       <c r="H45" s="35">
-        <f t="shared" ref="H45" si="39">MATCH("XX",H46:H57,0)</f>
+        <f t="shared" ref="H45" si="38">MATCH("XX",H46:H57,0)</f>
         <v>6</v>
       </c>
       <c r="I45" s="35">
-        <f t="shared" ref="I45" si="40">MATCH("XX",I46:I57,0)</f>
+        <f t="shared" ref="I45" si="39">MATCH("XX",I46:I57,0)</f>
         <v>7</v>
       </c>
       <c r="J45" s="35">
-        <f t="shared" ref="J45" si="41">MATCH("XX",J46:J57,0)</f>
+        <f t="shared" ref="J45" si="40">MATCH("XX",J46:J57,0)</f>
         <v>8</v>
       </c>
       <c r="K45" s="35">
-        <f t="shared" ref="K45" si="42">MATCH("XX",K46:K57,0)</f>
+        <f t="shared" ref="K45" si="41">MATCH("XX",K46:K57,0)</f>
         <v>9</v>
       </c>
       <c r="L45" s="35">
-        <f t="shared" ref="L45" si="43">MATCH("XX",L46:L57,0)</f>
+        <f t="shared" ref="L45" si="42">MATCH("XX",L46:L57,0)</f>
         <v>10</v>
       </c>
       <c r="M45" s="35">
-        <f t="shared" ref="M45" si="44">MATCH("XX",M46:M57,0)</f>
+        <f t="shared" ref="M45" si="43">MATCH("XX",M46:M57,0)</f>
         <v>11</v>
       </c>
       <c r="N45" s="35">
-        <f t="shared" ref="N45" si="45">MATCH("XX",N46:N57,0)</f>
+        <f t="shared" ref="N45" si="44">MATCH("XX",N46:N57,0)</f>
         <v>12</v>
       </c>
       <c r="O45" s="36" t="s">
@@ -9089,7 +9012,7 @@
       <c r="M46" s="41"/>
       <c r="N46" s="41"/>
       <c r="O46" s="42">
-        <f t="shared" ref="O46:O57" si="46">SUM(C46:N46)</f>
+        <f t="shared" ref="O46:O57" si="45">SUM(C46:N46)</f>
         <v>0</v>
       </c>
       <c r="P46" s="43">
@@ -9097,7 +9020,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="43">
-        <f t="shared" ref="Q46:Q57" si="47">COUNT(C46:N46)</f>
+        <f t="shared" ref="Q46:Q57" si="46">COUNT(C46:N46)</f>
         <v>0</v>
       </c>
       <c r="R46" s="52"/>
@@ -9216,15 +9139,15 @@
       <c r="M47" s="41"/>
       <c r="N47" s="41"/>
       <c r="O47" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="43">
+        <f t="shared" ref="P47:P57" si="47">SUM(S47:AD47)*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P47" s="43">
-        <f t="shared" ref="P47:P57" si="48">SUM(S47:AD47)*2</f>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R47" s="52"/>
@@ -9343,15 +9266,15 @@
       <c r="M48" s="41"/>
       <c r="N48" s="41"/>
       <c r="O48" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P48" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q48" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R48" s="52"/>
@@ -9470,15 +9393,15 @@
       <c r="M49" s="41"/>
       <c r="N49" s="41"/>
       <c r="O49" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P49" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q49" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R49" s="52"/>
@@ -9597,15 +9520,15 @@
       <c r="M50" s="41"/>
       <c r="N50" s="41"/>
       <c r="O50" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P50" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q50" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R50" s="52"/>
@@ -9724,15 +9647,15 @@
       <c r="M51" s="41"/>
       <c r="N51" s="41"/>
       <c r="O51" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P51" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P51" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R51" s="52"/>
@@ -9851,15 +9774,15 @@
       <c r="M52" s="41"/>
       <c r="N52" s="41"/>
       <c r="O52" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P52" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q52" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P52" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q52" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R52" s="52"/>
@@ -9978,15 +9901,15 @@
       <c r="M53" s="41"/>
       <c r="N53" s="41"/>
       <c r="O53" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P53" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q53" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P53" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q53" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R53" s="52"/>
@@ -10105,15 +10028,15 @@
       <c r="M54" s="41"/>
       <c r="N54" s="41"/>
       <c r="O54" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P54" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q54" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P54" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q54" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R54" s="52"/>
@@ -10232,15 +10155,15 @@
       <c r="M55" s="41"/>
       <c r="N55" s="41"/>
       <c r="O55" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P55" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q55" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P55" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q55" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R55" s="52"/>
@@ -10359,15 +10282,15 @@
       </c>
       <c r="N56" s="41"/>
       <c r="O56" s="42">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P56" s="43">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q56" s="43">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P56" s="43">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q56" s="43">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R56" s="52"/>
@@ -10486,15 +10409,15 @@
         <v>37</v>
       </c>
       <c r="O57" s="48">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="P57" s="49">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="Q57" s="49">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="P57" s="49">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="Q57" s="49">
-        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R57" s="52"/>
@@ -13725,7 +13648,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14014,7 +13937,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -14072,7 +13995,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -14100,7 +14023,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -14128,7 +14051,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -14156,7 +14079,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -14465,7 +14388,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:J10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14505,7 +14428,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -14555,7 +14478,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -14581,7 +14504,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -14607,7 +14530,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -14633,7 +14556,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -14659,7 +14582,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -14687,7 +14610,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -14744,7 +14667,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -14794,7 +14717,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -14822,7 +14745,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -14838,7 +14761,7 @@
         <v>57282</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J16" s="18">
         <v>1450</v>
@@ -14850,7 +14773,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -14878,7 +14801,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -15205,7 +15128,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15255,7 +15178,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15311,7 +15234,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -15337,7 +15260,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -15363,7 +15286,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -15389,7 +15312,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -15417,7 +15340,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -15429,7 +15352,7 @@
         <v>57282</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="18">
         <v>1450</v>
@@ -15445,7 +15368,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -15494,7 +15417,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -15552,7 +15475,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -15580,7 +15503,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -15608,7 +15531,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -15636,7 +15559,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -15945,7 +15868,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15995,7 +15918,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -16051,7 +15974,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -16077,7 +16000,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -16103,7 +16026,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -16129,7 +16052,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -16157,7 +16080,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -16185,7 +16108,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -16224,7 +16147,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16274,7 +16197,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -16302,7 +16225,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -16318,7 +16241,7 @@
         <v>57282</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J16" s="18">
         <v>1450</v>
@@ -16330,7 +16253,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -16358,7 +16281,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -16725,7 +16648,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -16775,7 +16698,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -16801,7 +16724,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -16827,7 +16750,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -16853,7 +16776,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -16873,7 +16796,7 @@
         <v>1731</v>
       </c>
       <c r="L8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -16882,7 +16805,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -16910,7 +16833,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -16926,7 +16849,7 @@
         <v>57282</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="18">
         <v>1450</v>
@@ -16977,7 +16900,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -17035,7 +16958,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -17063,7 +16986,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -17091,7 +17014,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -17119,7 +17042,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -17482,7 +17405,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -17642,7 +17565,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17692,7 +17615,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -17720,7 +17643,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -17748,7 +17671,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -17776,7 +17699,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -18103,7 +18026,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18157,7 +18080,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -18327,7 +18250,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18385,7 +18308,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -18413,7 +18336,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -18441,7 +18364,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -18469,7 +18392,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -18777,9 +18700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -18832,7 +18753,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -18992,7 +18913,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -19042,7 +18963,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -19070,7 +18991,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -19098,7 +19019,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -19126,7 +19047,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">

</xml_diff>